<commit_message>
DB Werkend, DB Gekoppeld aan admin
</commit_message>
<xml_diff>
--- a/Bestelformulier.xlsx
+++ b/Bestelformulier.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ALA\ALA Site\ALA-Versnelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207779C5-5214-43E8-8CF2-75400FCBEB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C96082B-F075-4812-9152-890F556B1487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2A3571CD-4E07-41C2-8874-12AF6664D2CF}"/>
   </bookViews>
@@ -466,7 +466,7 @@
     <t>Prijs</t>
   </si>
   <si>
-    <t>Thomas van Bruchem</t>
+    <t>Bart van Wijk</t>
   </si>
 </sst>
 </file>
@@ -674,6 +674,18 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -684,18 +696,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1070,7 +1070,7 @@
   <dimension ref="A1:G156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1117,9 +1117,9 @@
       <c r="B6" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
@@ -1128,11 +1128,11 @@
         <v>141</v>
       </c>
       <c r="B7" s="12">
-        <v>328734</v>
+        <v>79001</v>
       </c>
       <c r="C7" s="9"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
@@ -1141,22 +1141,22 @@
         <v>140</v>
       </c>
       <c r="B8" s="13">
-        <v>44614</v>
+        <v>44637</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
@@ -1183,7 +1183,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="14">
-        <v>230023</v>
+        <v>2</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="20">
@@ -1204,13 +1204,13 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
@@ -1263,9 +1263,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="7"/>
-      <c r="D17" s="14">
-        <v>32</v>
-      </c>
+      <c r="D17" s="14"/>
       <c r="E17" s="21">
         <v>1.54</v>
       </c>
@@ -1291,9 +1289,7 @@
         <v>10</v>
       </c>
       <c r="C19" s="7"/>
-      <c r="D19" s="14">
-        <v>34</v>
-      </c>
+      <c r="D19" s="14"/>
       <c r="E19" s="21">
         <v>1.63</v>
       </c>
@@ -1338,13 +1334,13 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
@@ -1477,9 +1473,7 @@
         <v>22</v>
       </c>
       <c r="C33" s="7"/>
-      <c r="D33" s="14">
-        <v>2</v>
-      </c>
+      <c r="D33" s="14"/>
       <c r="E33" s="21">
         <v>1.73</v>
       </c>
@@ -1530,9 +1524,7 @@
       <c r="B37" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="14">
-        <v>5</v>
-      </c>
+      <c r="C37" s="14"/>
       <c r="D37" s="7"/>
       <c r="E37" s="21">
         <v>0.35</v>
@@ -1559,9 +1551,7 @@
         <v>28</v>
       </c>
       <c r="C39" s="7"/>
-      <c r="D39" s="14">
-        <v>3</v>
-      </c>
+      <c r="D39" s="14"/>
       <c r="E39" s="21">
         <v>1.79</v>
       </c>
@@ -1599,7 +1589,9 @@
       <c r="B42" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="14"/>
+      <c r="C42" s="14">
+        <v>45</v>
+      </c>
       <c r="D42" s="7"/>
       <c r="E42" s="21">
         <v>0.69</v>
@@ -1664,9 +1656,7 @@
       <c r="B47" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C47" s="14">
-        <v>31</v>
-      </c>
+      <c r="C47" s="14"/>
       <c r="D47" s="7"/>
       <c r="E47" s="21">
         <v>1.49</v>
@@ -1771,9 +1761,7 @@
         <v>44</v>
       </c>
       <c r="C55" s="7"/>
-      <c r="D55" s="14">
-        <v>4</v>
-      </c>
+      <c r="D55" s="14"/>
       <c r="E55" s="21">
         <v>8.99</v>
       </c>
@@ -1786,7 +1774,9 @@
         <v>45</v>
       </c>
       <c r="C56" s="7"/>
-      <c r="D56" s="14"/>
+      <c r="D56" s="14">
+        <v>23</v>
+      </c>
       <c r="E56" s="21">
         <v>18.690000000000001</v>
       </c>
@@ -1805,13 +1795,13 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="22" t="s">
+      <c r="A58" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="B58" s="22"/>
-      <c r="C58" s="22"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="22"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
@@ -1890,9 +1880,7 @@
         <v>51</v>
       </c>
       <c r="C64" s="7"/>
-      <c r="D64" s="14">
-        <v>9</v>
-      </c>
+      <c r="D64" s="14"/>
       <c r="E64" s="21">
         <v>1.75</v>
       </c>
@@ -1905,9 +1893,7 @@
         <v>52</v>
       </c>
       <c r="C65" s="7"/>
-      <c r="D65" s="14">
-        <v>5</v>
-      </c>
+      <c r="D65" s="14"/>
       <c r="E65" s="21">
         <v>1.49</v>
       </c>
@@ -1984,9 +1970,7 @@
       <c r="B71" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C71" s="14">
-        <v>23</v>
-      </c>
+      <c r="C71" s="14"/>
       <c r="D71" s="7"/>
       <c r="E71" s="21">
         <v>0.69</v>
@@ -2052,7 +2036,7 @@
         <v>63</v>
       </c>
       <c r="C76" s="14">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="21">
@@ -2184,9 +2168,7 @@
         <v>73</v>
       </c>
       <c r="C86" s="7"/>
-      <c r="D86" s="14">
-        <v>35</v>
-      </c>
+      <c r="D86" s="14"/>
       <c r="E86" s="21">
         <v>1.49</v>
       </c>
@@ -2264,9 +2246,7 @@
         <v>79</v>
       </c>
       <c r="C92" s="7"/>
-      <c r="D92" s="14">
-        <v>4</v>
-      </c>
+      <c r="D92" s="14"/>
       <c r="E92" s="21">
         <v>2.99</v>
       </c>
@@ -2292,9 +2272,7 @@
         <v>81</v>
       </c>
       <c r="C94" s="7"/>
-      <c r="D94" s="14">
-        <v>23</v>
-      </c>
+      <c r="D94" s="14"/>
       <c r="E94" s="21">
         <v>7.69</v>
       </c>
@@ -2320,7 +2298,9 @@
         <v>83</v>
       </c>
       <c r="C96" s="7"/>
-      <c r="D96" s="14"/>
+      <c r="D96" s="14">
+        <v>25</v>
+      </c>
       <c r="E96" s="21">
         <v>1.25</v>
       </c>
@@ -2333,9 +2313,7 @@
         <v>84</v>
       </c>
       <c r="C97" s="7"/>
-      <c r="D97" s="14">
-        <v>53</v>
-      </c>
+      <c r="D97" s="14"/>
       <c r="E97" s="21">
         <v>0.89</v>
       </c>
@@ -2406,13 +2384,13 @@
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A103" s="22" t="s">
+      <c r="A103" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="B103" s="22"/>
-      <c r="C103" s="22"/>
-      <c r="D103" s="22"/>
-      <c r="E103" s="22"/>
+      <c r="B103" s="26"/>
+      <c r="C103" s="26"/>
+      <c r="D103" s="26"/>
+      <c r="E103" s="26"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
@@ -2478,7 +2456,9 @@
         <v>93</v>
       </c>
       <c r="C108" s="7"/>
-      <c r="D108" s="14"/>
+      <c r="D108" s="14">
+        <v>4</v>
+      </c>
       <c r="E108" s="21">
         <v>6.99</v>
       </c>
@@ -2491,9 +2471,7 @@
         <v>94</v>
       </c>
       <c r="C109" s="7"/>
-      <c r="D109" s="14">
-        <v>2</v>
-      </c>
+      <c r="D109" s="14"/>
       <c r="E109" s="21">
         <v>1.1499999999999999</v>
       </c>
@@ -2512,13 +2490,13 @@
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A111" s="22" t="s">
+      <c r="A111" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B111" s="22"/>
-      <c r="C111" s="22"/>
-      <c r="D111" s="22"/>
-      <c r="E111" s="22"/>
+      <c r="B111" s="26"/>
+      <c r="C111" s="26"/>
+      <c r="D111" s="26"/>
+      <c r="E111" s="26"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
@@ -2570,9 +2548,7 @@
       <c r="B115" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C115" s="14">
-        <v>6</v>
-      </c>
+      <c r="C115" s="14"/>
       <c r="D115" s="7"/>
       <c r="E115" s="21">
         <v>0.85</v>
@@ -2598,9 +2574,7 @@
       <c r="B117" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C117" s="14">
-        <v>35342</v>
-      </c>
+      <c r="C117" s="14"/>
       <c r="D117" s="7"/>
       <c r="E117" s="21">
         <v>1.45</v>
@@ -2652,9 +2626,7 @@
       <c r="B121" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C121" s="14">
-        <v>54</v>
-      </c>
+      <c r="C121" s="14"/>
       <c r="D121" s="7"/>
       <c r="E121" s="21">
         <v>0.99</v>
@@ -2694,9 +2666,7 @@
         <v>107</v>
       </c>
       <c r="C124" s="7"/>
-      <c r="D124" s="14">
-        <v>6</v>
-      </c>
+      <c r="D124" s="14"/>
       <c r="E124" s="21">
         <v>2.99</v>
       </c>
@@ -2741,13 +2711,13 @@
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A128" s="23" t="s">
+      <c r="A128" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="B128" s="24"/>
-      <c r="C128" s="24"/>
-      <c r="D128" s="24"/>
-      <c r="E128" s="25"/>
+      <c r="B128" s="28"/>
+      <c r="C128" s="28"/>
+      <c r="D128" s="28"/>
+      <c r="E128" s="29"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
@@ -2800,9 +2770,7 @@
         <v>113</v>
       </c>
       <c r="C132" s="7"/>
-      <c r="D132" s="14">
-        <v>32483</v>
-      </c>
+      <c r="D132" s="14"/>
       <c r="E132" s="21">
         <v>2.25</v>
       </c>
@@ -2880,7 +2848,9 @@
         <v>119</v>
       </c>
       <c r="C138" s="7"/>
-      <c r="D138" s="14"/>
+      <c r="D138" s="14">
+        <v>23</v>
+      </c>
       <c r="E138" s="21">
         <v>4.99</v>
       </c>
@@ -2893,9 +2863,7 @@
         <v>120</v>
       </c>
       <c r="C139" s="7"/>
-      <c r="D139" s="14">
-        <v>3432</v>
-      </c>
+      <c r="D139" s="14"/>
       <c r="E139" s="21">
         <v>1.7</v>
       </c>
@@ -2908,9 +2876,7 @@
         <v>121</v>
       </c>
       <c r="C140" s="7"/>
-      <c r="D140" s="14">
-        <v>11109</v>
-      </c>
+      <c r="D140" s="14"/>
       <c r="E140" s="21">
         <v>11.99</v>
       </c>
@@ -2988,9 +2954,7 @@
         <v>127</v>
       </c>
       <c r="C146" s="7"/>
-      <c r="D146" s="14">
-        <v>598</v>
-      </c>
+      <c r="D146" s="14"/>
       <c r="E146" s="21">
         <v>1.56</v>
       </c>
@@ -3015,9 +2979,7 @@
       <c r="B148" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="C148" s="14">
-        <v>1832</v>
-      </c>
+      <c r="C148" s="14"/>
       <c r="D148" s="7"/>
       <c r="E148" s="21">
         <v>0.56000000000000005</v>
@@ -3068,17 +3030,18 @@
       <c r="B156" s="2"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="qD9/fbH1/AoFXgNgI5aWf7fS8/HysAp1DejrEK7uMacHJ15Vq7N+h3ESDBmsJGlYKJupgfMXXwTexJtL/y1cGA==" saltValue="58eXoarfYO+qu6C9vN2mfg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="10">
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A103:E103"/>
+    <mergeCell ref="A111:E111"/>
+    <mergeCell ref="A128:E128"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A103:E103"/>
-    <mergeCell ref="A111:E111"/>
-    <mergeCell ref="A128:E128"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>